<commit_message>
Day-4-Second-Commit-Verification of failed new profile addition
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Apollo User Inputs.xlsx
+++ b/src/test/resources/Exceldata/Apollo User Inputs.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A1E6DBF9-D2FB-4814-AEA7-486B1CA36A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Sprint Implementation\Apollo247TestingApp\src\test\resources\Exceldata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576CF43-260D-4940-BC96-F3D0EE94E4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2988" yWindow="2100" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -51,16 +55,42 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Email-id</t>
+  </si>
+  <si>
+    <t>alice@gmail.com</t>
+  </si>
+  <si>
+    <t>12Alice</t>
+  </si>
+  <si>
+    <t>$K</t>
+  </si>
+  <si>
+    <t>99-99-9999</t>
+  </si>
+  <si>
+    <t>alice.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,14 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,7 +416,7 @@
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +435,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9176226906</v>
       </c>
@@ -422,13 +458,36 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2654965</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9176226906</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{7FDB4680-8C40-49F3-80D3-6F04C8B60D9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-6-Second-Commit-Verification of BMI for weight management
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Apollo User Inputs.xlsx
+++ b/src/test/resources/Exceldata/Apollo User Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Sprint Implementation\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576CF43-260D-4940-BC96-F3D0EE94E4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CEB1E6-17F4-4317-BC92-77F3F8E24D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2988" yWindow="2100" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>alice.com</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,7 +422,7 @@
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +444,14 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9176226906</v>
       </c>
@@ -461,13 +473,25 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H2">
+        <v>-170</v>
+      </c>
+      <c r="I2">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2654965</v>
       </c>
+      <c r="H3">
+        <v>160</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9176226906</v>
       </c>
@@ -482,6 +506,28 @@
       </c>
       <c r="G4" t="s">
         <v>15</v>
+      </c>
+      <c r="H4">
+        <v>168468</v>
+      </c>
+      <c r="I4">
+        <v>54684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>180</v>
+      </c>
+      <c r="I5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>150.9</v>
+      </c>
+      <c r="I6">
+        <v>56.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>